<commit_message>
Search api only once for faster results
</commit_message>
<xml_diff>
--- a/StockScreener.xlsx
+++ b/StockScreener.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kathan\PycharmProjects\StockScreener\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922C6396-D5F0-4E5F-B63C-B2A47880AEBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF30D7EB-EEF3-4DCF-B9F9-16896446BC62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="90" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="companylist" sheetId="1" r:id="rId1"/>
@@ -16819,8 +16819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A10163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection sqref="A1:A5311"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>